<commit_message>
DEMO with save button VERSION 2 (adding check before DO)
</commit_message>
<xml_diff>
--- a/ISUZU_template.xlsx
+++ b/ISUZU_template.xlsx
@@ -50100,7 +50100,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -50132,48 +50132,18 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="22" t="inlineStr">
+      <c r="A2" t="inlineStr">
         <is>
           <t>設備ｾﾝﾀｰ</t>
         </is>
       </c>
-      <c r="B2" s="22" t="inlineStr">
+      <c r="B2" t="inlineStr">
         <is>
           <t>J08002</t>
         </is>
       </c>
-      <c r="C2" s="22" t="n">
+      <c r="C2" t="n">
         <v>3</v>
-      </c>
-      <c r="D2" s="22" t="inlineStr">
-        <is>
-          <t>Done 12 months without error !</t>
-        </is>
-      </c>
-      <c r="E2" s="22" t="inlineStr">
-        <is>
-          <t>Done 12 months without error !</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="22" t="inlineStr">
-        <is>
-          <t>OBP設備ｾﾝﾀｰ</t>
-        </is>
-      </c>
-      <c r="B3" s="22" t="inlineStr">
-        <is>
-          <t>J08000</t>
-        </is>
-      </c>
-      <c r="C3" s="22" t="n">
-        <v>3</v>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>Done 12 months without error !</t>
-        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>